<commit_message>
added a brief Verification Plan for this repo
</commit_message>
<xml_diff>
--- a/docs/VerifPlan.xlsx
+++ b/docs/VerifPlan.xlsx
@@ -63,43 +63,43 @@
     <t>Constrained-Random</t>
   </si>
   <si>
+    <t>Assertion Coverage</t>
+  </si>
+  <si>
+    <t>https://github.com/npatsiatzis/fizzbuzz/blob/main/pyuvm_sim/coverage.xml</t>
+  </si>
+  <si>
+    <t>(number %5 == 0) |-&gt; buzz==1</t>
+  </si>
+  <si>
+    <t>When the number is divisible by 5 the output fizz should be active</t>
+  </si>
+  <si>
+    <t>Verify this property dynamically (in simulation) for all possible combination of input space (cross product)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- END -----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>RISC-V Compliance</t>
+  </si>
+  <si>
+    <t>Testcase</t>
+  </si>
+  <si>
+    <t>Signature Check</t>
+  </si>
+  <si>
+    <t>OpenHW Compliance</t>
+  </si>
+  <si>
     <t>Functional Coverage</t>
   </si>
   <si>
-    <t>https://github.com/npatsiatzis/simple_adder/blob/main/pyuvm_sim/coverage_pyuvm.xml</t>
-  </si>
-  <si>
-    <t>(number %5 == 0) |-&gt; buzz==1</t>
-  </si>
-  <si>
-    <t>When the number is divisible by 5 the output fizz should be active</t>
-  </si>
-  <si>
-    <t>Verify this property dynamically (in simulation) for all possible combination of input space (cross product)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- END -----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------</t>
-  </si>
-  <si>
-    <t>RISC-V Compliance</t>
-  </si>
-  <si>
-    <t>Testcase</t>
-  </si>
-  <si>
-    <t>Signature Check</t>
-  </si>
-  <si>
-    <t>OpenHW Compliance</t>
-  </si>
-  <si>
     <t>Check against RM</t>
   </si>
   <si>
     <t>Directed Self-Checking</t>
-  </si>
-  <si>
-    <t>Assertion Coverage</t>
   </si>
   <si>
     <t>Assertion Check</t>
@@ -163,6 +163,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -179,14 +187,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -629,7 +629,7 @@
     <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -638,10 +638,10 @@
     <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -650,7 +650,7 @@
     <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -659,7 +659,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -668,19 +668,19 @@
     <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -695,7 +695,7 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -705,7 +705,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
@@ -733,7 +733,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -743,25 +743,25 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -785,7 +785,8 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="48" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1178,10 +1179,10 @@
   <sheetPr/>
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.0074074074074" defaultRowHeight="14.25"/>
@@ -1276,7 +1277,7 @@
       <c r="H3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="12" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1289,7 +1290,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="11"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" s="3" customFormat="1" spans="1:9">
       <c r="A5" s="8"/>
@@ -2143,17 +2144,17 @@
       <c r="I83" s="8"/>
     </row>
     <row r="84" s="4" customFormat="1" spans="1:9">
-      <c r="A84" s="12" t="s">
+      <c r="A84" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B84" s="12"/>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-      <c r="I84" s="12"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2171,8 +2172,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" display="https://github.com/npatsiatzis/simple_adder/blob/main/pyuvm_sim/coverage_pyuvm.xml"/>
-    <hyperlink ref="I3" r:id="rId1" display="https://github.com/npatsiatzis/simple_adder/blob/main/pyuvm_sim/coverage_pyuvm.xml"/>
+    <hyperlink ref="I2" r:id="rId1" display="https://github.com/npatsiatzis/fizzbuzz/blob/main/pyuvm_sim/coverage.xml" tooltip="https://github.com/npatsiatzis/fizzbuzz/blob/main/pyuvm_sim/coverage.xml"/>
+    <hyperlink ref="I3" r:id="rId1" display="https://github.com/npatsiatzis/fizzbuzz/blob/main/pyuvm_sim/coverage.xml" tooltip="https://github.com/npatsiatzis/fizzbuzz/blob/main/pyuvm_sim/coverage.xml"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -2228,18 +2229,18 @@
         <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5">

</xml_diff>